<commit_message>
corrección de clusters y preguntas de exploracion.
</commit_message>
<xml_diff>
--- a/df_clusterizado.xlsx
+++ b/df_clusterizado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92ca9ff1cf61ae79/Escritorio/data mining/Proyecto_2/Proyecto_unsupervised_learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{F0CDBC4A-02FF-4167-9C64-E8497FF283C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E75058E7-16E8-4A28-814A-0D426E26BC4F}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{F0CDBC4A-02FF-4167-9C64-E8497FF283C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1013DF54-09E7-411F-A874-8C50A2A6E99B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B61F6142-860F-4F03-9638-0AC729C393F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{B61F6142-860F-4F03-9638-0AC729C393F9}"/>
   </bookViews>
   <sheets>
     <sheet name="df_clusterizado" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -11308,7 +11308,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{164FCDAE-D2FF-43E0-9EDF-38C2778324C7}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{164FCDAE-D2FF-43E0-9EDF-38C2778324C7}" name="TablaDinámica2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:H3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" showAll="0">
@@ -11740,7 +11740,450 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{58E228DF-FBFE-45D3-A467-8C30CDC0AC7B}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{76A5B539-F12D-4F0A-9B28-1DCC6B90B7DF}" name="TablaDinámica4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A19:E26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0">
+      <items count="51">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="51">
+        <item x="0"/>
+        <item x="44"/>
+        <item x="47"/>
+        <item x="1"/>
+        <item x="26"/>
+        <item x="2"/>
+        <item x="34"/>
+        <item x="37"/>
+        <item x="40"/>
+        <item x="3"/>
+        <item x="41"/>
+        <item x="4"/>
+        <item x="43"/>
+        <item x="38"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="36"/>
+        <item x="7"/>
+        <item x="39"/>
+        <item x="8"/>
+        <item x="48"/>
+        <item x="27"/>
+        <item x="9"/>
+        <item x="31"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="35"/>
+        <item x="28"/>
+        <item x="49"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="29"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="45"/>
+        <item x="25"/>
+        <item x="30"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="42"/>
+        <item x="33"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="32"/>
+        <item x="46"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="33">
+        <item x="19"/>
+        <item x="5"/>
+        <item x="31"/>
+        <item x="0"/>
+        <item x="16"/>
+        <item x="2"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="28"/>
+        <item x="8"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="29"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="30"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="13"/>
+        <item x="27"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="51">
+        <item x="25"/>
+        <item x="0"/>
+        <item x="46"/>
+        <item x="11"/>
+        <item x="30"/>
+        <item x="36"/>
+        <item x="34"/>
+        <item x="12"/>
+        <item x="27"/>
+        <item x="40"/>
+        <item x="28"/>
+        <item x="43"/>
+        <item x="45"/>
+        <item x="26"/>
+        <item x="42"/>
+        <item x="8"/>
+        <item x="33"/>
+        <item x="5"/>
+        <item x="32"/>
+        <item x="37"/>
+        <item x="31"/>
+        <item x="47"/>
+        <item x="49"/>
+        <item x="19"/>
+        <item x="38"/>
+        <item x="4"/>
+        <item x="48"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="39"/>
+        <item x="41"/>
+        <item x="35"/>
+        <item x="23"/>
+        <item x="16"/>
+        <item x="9"/>
+        <item x="44"/>
+        <item x="29"/>
+        <item x="14"/>
+        <item x="3"/>
+        <item x="24"/>
+        <item x="15"/>
+        <item x="21"/>
+        <item x="10"/>
+        <item x="22"/>
+        <item x="1"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="1"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="13"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Promedio de rebounds_per_game" fld="4" subtotal="average" baseField="13" baseItem="0"/>
+    <dataField name="Promedio de age" fld="2" subtotal="average" baseField="13" baseItem="0"/>
+    <dataField name="Promedio de assists_per_game" fld="5" subtotal="average" baseField="13" baseItem="0"/>
+    <dataField name="Promedio de points_per_game" fld="6" subtotal="average" baseField="13" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="13">
+    <chartFormat chart="5" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{58E228DF-FBFE-45D3-A467-8C30CDC0AC7B}" name="TablaDinámica3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A1:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0">
@@ -12332,449 +12775,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{76A5B539-F12D-4F0A-9B28-1DCC6B90B7DF}" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A19:E26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0">
-      <items count="51">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="51">
-        <item x="0"/>
-        <item x="44"/>
-        <item x="47"/>
-        <item x="1"/>
-        <item x="26"/>
-        <item x="2"/>
-        <item x="34"/>
-        <item x="37"/>
-        <item x="40"/>
-        <item x="3"/>
-        <item x="41"/>
-        <item x="4"/>
-        <item x="43"/>
-        <item x="38"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="36"/>
-        <item x="7"/>
-        <item x="39"/>
-        <item x="8"/>
-        <item x="48"/>
-        <item x="27"/>
-        <item x="9"/>
-        <item x="31"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="35"/>
-        <item x="28"/>
-        <item x="49"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="29"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="45"/>
-        <item x="25"/>
-        <item x="30"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="42"/>
-        <item x="33"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="32"/>
-        <item x="46"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="33">
-        <item x="19"/>
-        <item x="5"/>
-        <item x="31"/>
-        <item x="0"/>
-        <item x="16"/>
-        <item x="2"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="28"/>
-        <item x="8"/>
-        <item x="25"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="29"/>
-        <item x="11"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="30"/>
-        <item x="12"/>
-        <item x="10"/>
-        <item x="13"/>
-        <item x="27"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="18"/>
-        <item x="14"/>
-        <item x="1"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="51">
-        <item x="25"/>
-        <item x="0"/>
-        <item x="46"/>
-        <item x="11"/>
-        <item x="30"/>
-        <item x="36"/>
-        <item x="34"/>
-        <item x="12"/>
-        <item x="27"/>
-        <item x="40"/>
-        <item x="28"/>
-        <item x="43"/>
-        <item x="45"/>
-        <item x="26"/>
-        <item x="42"/>
-        <item x="8"/>
-        <item x="33"/>
-        <item x="5"/>
-        <item x="32"/>
-        <item x="37"/>
-        <item x="31"/>
-        <item x="47"/>
-        <item x="49"/>
-        <item x="19"/>
-        <item x="38"/>
-        <item x="4"/>
-        <item x="48"/>
-        <item x="2"/>
-        <item x="7"/>
-        <item x="39"/>
-        <item x="41"/>
-        <item x="35"/>
-        <item x="23"/>
-        <item x="16"/>
-        <item x="9"/>
-        <item x="44"/>
-        <item x="29"/>
-        <item x="14"/>
-        <item x="3"/>
-        <item x="24"/>
-        <item x="15"/>
-        <item x="21"/>
-        <item x="10"/>
-        <item x="22"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="20"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item sd="0" x="0"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="1"/>
-        <item t="default" sd="0"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="13"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="4">
-    <dataField name="Promedio de rebounds_per_game" fld="4" subtotal="average" baseField="13" baseItem="0"/>
-    <dataField name="Promedio de age" fld="2" subtotal="average" baseField="13" baseItem="0"/>
-    <dataField name="Promedio de assists_per_game" fld="5" subtotal="average" baseField="13" baseItem="0"/>
-    <dataField name="Promedio de points_per_game" fld="6" subtotal="average" baseField="13" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="13">
-    <chartFormat chart="5" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="11" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="18" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -13094,7 +13094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5325BA71-8AED-4306-B8F5-98E33613C031}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17:H18"/>
     </sheetView>
   </sheetViews>
@@ -15495,7 +15495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D4DD31-98BF-4D21-8B68-32B7BA6EC8EC}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="101" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>